<commit_message>
add figures, update charts code
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohan\Documents\EPQ charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\selva\Documents\Coding\EPQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B8C919-C1E8-4A26-9E66-C0CF6599FDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF22FE8-1E41-467D-BDFD-0DA9E6FFBB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{92BFCFC7-AC86-46C9-9D17-467961656618}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{92BFCFC7-AC86-46C9-9D17-467961656618}"/>
   </bookViews>
   <sheets>
     <sheet name="admissions" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="197">
   <si>
     <t>QueenMary, University of Lon.. Other Russell Group</t>
   </si>
@@ -517,9 +517,6 @@
   </si>
   <si>
     <t>English Literature</t>
-  </si>
-  <si>
-    <t>English Language &amp; Literature</t>
   </si>
   <si>
     <t>subject</t>
@@ -1067,10 +1064,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1205,16 +1202,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1228,7 +1225,7 @@
         <v>1.9713782072067261</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,7 +1239,7 @@
         <v>1.0964227914810181</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,7 +1253,7 @@
         <v>1.5937222242355347</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,7 +1267,7 @@
         <v>1.0641186237335205</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1284,7 +1281,7 @@
         <v>1.0305472612380981</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1298,7 +1295,7 @@
         <v>1.5636910200119019</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,7 +1309,7 @@
         <v>1.0903264284133911</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,7 +1323,7 @@
         <v>1.3240159749984741</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,7 +1337,7 @@
         <v>0.82732939720153809</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1354,7 +1351,7 @@
         <v>1.7760151624679565</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1368,7 +1365,7 @@
         <v>1.0113992691040039</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1382,7 +1379,7 @@
         <v>1.2662296295166016</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,7 +1393,7 @@
         <v>0.90979486703872681</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,7 +1407,7 @@
         <v>1.1499499082565308</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,7 +1435,7 @@
         <v>1.0530462265014648</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,7 +1449,7 @@
         <v>1.1343294382095337</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,7 +1463,7 @@
         <v>1.5071463584899902</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,7 +1477,7 @@
         <v>1.7356675863265991</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1494,7 +1491,7 @@
         <v>1.576213002204895</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,7 +1505,7 @@
         <v>2.0234951972961426</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,7 +1519,7 @@
         <v>1.397850513458252</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,7 +1533,7 @@
         <v>1.7692694664001465</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1550,7 +1547,7 @@
         <v>1.4011307954788208</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,7 +1561,7 @@
         <v>1.3458186388015747</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1578,7 +1575,7 @@
         <v>0.95078802108764648</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1592,7 +1589,7 @@
         <v>1.662558913230896</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,7 +1603,7 @@
         <v>0.98858988285064697</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,7 +1617,7 @@
         <v>1.1802462339401245</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,7 +1631,7 @@
         <v>1.9633474349975586</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,7 +1645,7 @@
         <v>2.9633908271789551</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1658,11 +1655,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8DA5E3-C5AF-4EA3-A423-ADB8D65E05D0}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L123" sqref="L123"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,33 +1669,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" s="7">
-        <v>1.2999999999999999E-2</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="D2" s="7">
-        <v>0.625</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -1707,16 +1703,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C3" s="7">
-        <v>4.5999999999999999E-2</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="D3" s="8">
-        <v>0.61099999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -1724,16 +1720,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C4" s="7">
-        <v>3.7999999999999999E-2</v>
+        <v>0.246</v>
       </c>
       <c r="D4" s="7">
-        <v>0.60299999999999998</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -1741,16 +1737,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C5" s="7">
-        <v>8.9999999999999993E-3</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="D5" s="7">
-        <v>0.59</v>
+        <v>0.25</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -1758,222 +1754,220 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>185</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C6" s="7">
-        <v>0.01</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="D6" s="7">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C7" s="7">
-        <v>5.8999999999999997E-2</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="D7" s="7">
-        <v>0.498</v>
+        <v>0.191</v>
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C8" s="7">
-        <v>1.2E-2</v>
+        <v>0.2</v>
       </c>
       <c r="D8" s="7">
-        <v>0.48899999999999999</v>
+        <v>0.248</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C9" s="7">
-        <v>1.4999999999999999E-2</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="D9" s="7">
-        <v>0.46100000000000002</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="7">
-        <v>4.2999999999999997E-2</v>
+        <v>0.161</v>
       </c>
       <c r="D10" s="7">
-        <v>0.45500000000000002</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C11" s="7">
-        <v>0.01</v>
+        <v>0.151</v>
       </c>
       <c r="D11" s="7">
-        <v>0.42299999999999999</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C12" s="7">
-        <v>0.161</v>
+        <v>0.15</v>
       </c>
       <c r="D12" s="7">
-        <v>0.42199999999999999</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C13" s="7">
-        <v>1.6E-2</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="D13" s="7">
-        <v>0.42199999999999999</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C14" s="7">
-        <v>0.104</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="D14" s="7">
-        <v>0.41899999999999998</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C15" s="7">
-        <v>2.3E-2</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="D15" s="7">
-        <v>0.40899999999999997</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C16" s="7">
-        <v>3.3000000000000002E-2</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="D16" s="7">
-        <v>0.4</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C17" s="7">
-        <v>1.4999999999999999E-2</v>
+        <v>0.126</v>
       </c>
       <c r="D17" s="7">
-        <v>0.39800000000000002</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C18" s="7">
-        <v>1.4E-2</v>
+        <v>0.124</v>
       </c>
       <c r="D18" s="7">
-        <v>0.38800000000000001</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C19" s="7">
-        <v>3.5000000000000003E-2</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="D19" s="7">
-        <v>0.38400000000000001</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="7">
         <v>0.11600000000000001</v>
@@ -1983,1401 +1977,1400 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C21" s="7">
-        <v>1.4999999999999999E-2</v>
+        <v>0.109</v>
       </c>
       <c r="D21" s="7">
-        <v>0.36799999999999999</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="7">
-        <v>0.01</v>
+        <v>0.108</v>
       </c>
       <c r="D22" s="7">
-        <v>0.36799999999999999</v>
+        <v>0.28699999999999998</v>
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" s="7">
-        <v>3.5999999999999997E-2</v>
+        <v>0.104</v>
       </c>
       <c r="D23" s="7">
-        <v>0.36199999999999999</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="7">
-        <v>2.8000000000000001E-2</v>
+        <v>0.104</v>
       </c>
       <c r="D24" s="7">
-        <v>0.36199999999999999</v>
+        <v>0.314</v>
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" s="7">
-        <v>0.15</v>
+        <v>0.104</v>
       </c>
       <c r="D25" s="7">
-        <v>0.35099999999999998</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="7">
-        <v>2.9000000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D26" s="7">
-        <v>0.34300000000000003</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C27" s="7">
-        <v>1.7999999999999999E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D27" s="7">
-        <v>0.33800000000000002</v>
+        <v>0.122</v>
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C28" s="7">
-        <v>3.2000000000000001E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D28" s="7">
-        <v>0.32500000000000001</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C29" s="7">
-        <v>2.4E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="D29" s="7">
-        <v>0.32500000000000001</v>
+        <v>0.122</v>
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C30" s="7">
-        <v>1.7999999999999999E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="D30" s="7">
-        <v>0.32</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C31" s="7">
-        <v>0.104</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="D31" s="7">
-        <v>0.314</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="7">
-        <v>3.7999999999999999E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="D32" s="7">
-        <v>0.314</v>
+        <v>0.189</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C33" s="7">
-        <v>3.5999999999999997E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D33" s="7">
-        <v>0.314</v>
+        <v>0.153</v>
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C34" s="7">
-        <v>3.2000000000000001E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D34" s="7">
-        <v>0.30099999999999999</v>
+        <v>0.108</v>
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C35" s="7">
-        <v>3.6999999999999998E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="D35" s="7">
-        <v>0.29799999999999999</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C36" s="7">
-        <v>5.8999999999999997E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D36" s="7">
-        <v>0.29499999999999998</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C37" s="7">
-        <v>0.13900000000000001</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D37" s="7">
-        <v>0.28899999999999998</v>
+        <v>0.106</v>
       </c>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C38" s="7">
-        <v>0.104</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="D38" s="7">
-        <v>0.28899999999999998</v>
+        <v>0.17</v>
       </c>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C39" s="7">
-        <v>0.108</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D39" s="7">
-        <v>0.28699999999999998</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C40" s="7">
-        <v>1.2E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D40" s="7">
-        <v>0.28399999999999997</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="7">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.115</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="7">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.498</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="7">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="7">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" s="7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.151</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="7">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D49" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="7">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="7">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C52" s="7">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D52" s="7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" s="7">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C54" s="7">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D54" s="7">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" s="7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.153</v>
+      </c>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" s="7">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C58" s="7">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D58" s="7">
+        <v>0.184</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" s="7">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C41" s="7">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C42" s="7">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" s="7">
-        <v>1.2E-2</v>
-      </c>
-      <c r="D43" s="7">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C44" s="7">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="D44" s="7">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" s="7">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="D45" s="7">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C46" s="7">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="D46" s="7">
-        <v>0.255</v>
-      </c>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="7">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="D47" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C48" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D48" s="7">
-        <v>0.248</v>
-      </c>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C49" s="7">
-        <v>2.4E-2</v>
-      </c>
-      <c r="D49" s="7">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C50" s="7">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D50" s="7">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C51" s="7">
-        <v>0.06</v>
-      </c>
-      <c r="D51" s="7">
-        <v>0.23699999999999999</v>
-      </c>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C52" s="7">
-        <v>2.7E-2</v>
-      </c>
-      <c r="D52" s="7">
-        <v>0.23699999999999999</v>
-      </c>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C53" s="7">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="D53" s="7">
-        <v>0.23</v>
-      </c>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C54" s="7">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="D54" s="7">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="7">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="D55" s="7">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C56" s="7">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D56" s="7">
-        <v>0.217</v>
-      </c>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" s="7">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="D57" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C58" s="7">
-        <v>0.109</v>
-      </c>
-      <c r="D58" s="7">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C59" s="7">
-        <v>3.1E-2</v>
-      </c>
-      <c r="D59" s="7">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="C60" s="7">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D60" s="7">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D61" s="7">
+        <v>0.314</v>
+      </c>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D62" s="7">
+        <v>0.255</v>
+      </c>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" s="7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.23</v>
+      </c>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" s="7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D64" s="7">
         <v>0.19900000000000001</v>
       </c>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B61" s="2" t="s">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C61" s="7">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D61" s="7">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C62" s="7">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="D62" s="7">
-        <v>0.192</v>
-      </c>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C63" s="7">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="D63" s="7">
-        <v>0.191</v>
-      </c>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C64" s="7">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="D64" s="7">
-        <v>0.189</v>
-      </c>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="C65" s="7">
-        <v>4.2999999999999997E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D65" s="7">
-        <v>0.184</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C66" s="7">
-        <v>0.03</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D66" s="7">
-        <v>0.184</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C67" s="7">
-        <v>2.9000000000000001E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D67" s="7">
-        <v>0.182</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C68" s="7">
-        <v>0.25700000000000001</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D68" s="7">
-        <v>0.18</v>
-      </c>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C69" s="7">
-        <v>4.7E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D69" s="7">
-        <v>0.17699999999999999</v>
+        <v>0.314</v>
       </c>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C70" s="7">
-        <v>6.9000000000000006E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D70" s="7">
-        <v>0.17</v>
+        <v>0.155</v>
       </c>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C71" s="7">
-        <v>0.1</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D71" s="7">
-        <v>0.16900000000000001</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C72" s="7">
-        <v>6.7000000000000004E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D72" s="7">
-        <v>0.16700000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C73" s="7">
-        <v>3.6999999999999998E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D73" s="7">
-        <v>0.16700000000000001</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C74" s="7">
-        <v>2.7E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="D74" s="7">
-        <v>0.16700000000000001</v>
+        <v>0.217</v>
       </c>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C75" s="7">
-        <v>8.1000000000000003E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="D75" s="7">
-        <v>0.16600000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C76" s="7">
-        <v>3.6999999999999998E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="D76" s="7">
-        <v>0.16500000000000001</v>
+        <v>0.107</v>
       </c>
       <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C77" s="7">
-        <v>0.246</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D77" s="7">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="E77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C78" s="7">
-        <v>0.20300000000000001</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D78" s="7">
-        <v>0.16400000000000001</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C79" s="7">
-        <v>3.5999999999999997E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D79" s="7">
-        <v>0.155</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C80" s="7">
-        <v>8.5000000000000006E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D80" s="7">
-        <v>0.153</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C81" s="7">
-        <v>4.3999999999999997E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D81" s="7">
-        <v>0.153</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C82" s="7">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="D82" s="7">
-        <v>0.151</v>
+        <v>0.184</v>
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C83" s="7">
-        <v>4.9000000000000002E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D83" s="7">
-        <v>0.14899999999999999</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C84" s="7">
-        <v>0.16800000000000001</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D84" s="7">
-        <v>0.14499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="E84" s="2"/>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C85" s="7">
-        <v>7.6999999999999999E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D85" s="7">
-        <v>0.14399999999999999</v>
+        <v>0.182</v>
       </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C86" s="7">
-        <v>0.151</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D86" s="7">
-        <v>0.13900000000000001</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C87" s="7">
-        <v>0.29499999999999998</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D87" s="7">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="E87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C88" s="7">
-        <v>8.6999999999999994E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D88" s="7">
-        <v>0.13800000000000001</v>
+        <v>0.23699999999999999</v>
       </c>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C89" s="7">
-        <v>0.126</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D89" s="7">
-        <v>0.13500000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C90" s="7">
-        <v>5.0999999999999997E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D90" s="7">
-        <v>0.13300000000000001</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C91" s="7">
-        <v>0.13900000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D91" s="7">
-        <v>0.13200000000000001</v>
+        <v>0.24399999999999999</v>
       </c>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C92" s="7">
-        <v>3.1E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D92" s="7">
-        <v>0.13200000000000001</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C93" s="7">
-        <v>9.8000000000000004E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D93" s="7">
-        <v>0.122</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C94" s="7">
-        <v>8.8999999999999996E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D94" s="7">
-        <v>0.122</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C95" s="7">
-        <v>6.8000000000000005E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D95" s="7">
-        <v>0.11899999999999999</v>
+        <v>0.104</v>
       </c>
       <c r="E95" s="2"/>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C96" s="7">
-        <v>0.13100000000000001</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D96" s="7">
-        <v>0.11600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E96" s="2"/>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C97" s="7">
-        <v>0.06</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D97" s="7">
-        <v>0.115</v>
+        <v>0</v>
       </c>
       <c r="E97" s="2"/>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C98" s="7">
-        <v>8.3000000000000004E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="D98" s="7">
-        <v>0.108</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="E98" s="2"/>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C99" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D99" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C100" s="7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D100" s="7">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C101" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D101" s="7">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C102" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D102" s="7">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C103" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D103" s="7">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C104" s="7">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D104" s="7">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C99" s="7">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="D99" s="7">
-        <v>0.107</v>
-      </c>
-      <c r="E99" s="2"/>
-    </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C100" s="7">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="D100" s="7">
-        <v>0.106</v>
-      </c>
-      <c r="E100" s="2"/>
-    </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C101" s="7">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D101" s="7">
-        <v>0.104</v>
-      </c>
-      <c r="E101" s="2"/>
-    </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C102" s="7">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="D102" s="7">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="E102" s="2"/>
-    </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C103" s="7">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="D103" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E103" s="2"/>
-    </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C104" s="7">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D104" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E104" s="2"/>
-    </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C105" s="7">
-        <v>9.8000000000000004E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D105" s="7">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="E105" s="2"/>
-    </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.625</v>
+      </c>
+      <c r="E105" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C106" s="7">
-        <v>3.5000000000000003E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D106" s="7">
-        <v>8.3000000000000004E-2</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="E106" s="2"/>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C107" s="7">
-        <v>3.1E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D107" s="7">
-        <v>8.3000000000000004E-2</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="E107" s="2"/>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C108" s="7">
-        <v>6.8000000000000005E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D108" s="7">
-        <v>8.2000000000000003E-2</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="E108" s="2"/>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>100</v>
+        <v>184</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C109" s="7">
-        <v>2.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D109" s="7">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="E109" s="2"/>
-    </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="E109" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C110" s="7">
-        <v>4.7E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D110" s="7">
-        <v>6.3E-2</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="E110" s="2"/>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C111" s="7">
-        <v>0.124</v>
+        <v>0.01</v>
       </c>
       <c r="D111" s="7">
-        <v>5.8000000000000003E-2</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="E111" s="2"/>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C112" s="7">
-        <v>2.1000000000000001E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D112" s="7">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2"/>
+        <v>0.59</v>
+      </c>
+      <c r="E112" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E112" xr:uid="{3C8DA5E3-C5AF-4EA3-A423-ADB8D65E05D0}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E112">
-      <sortCondition descending="1" ref="D1"/>
+      <sortCondition descending="1" ref="C1:C112"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3390,7 +3383,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,10 +3393,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3511,12 +3504,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.52</v>
-      </c>
+      <c r="B15" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B15" xr:uid="{25CEC08D-DC40-4426-BCE6-720A06971A90}">
@@ -3540,10 +3528,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C1">
         <v>2014</v>
@@ -3578,7 +3566,7 @@
         <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2">
         <v>110882</v>
@@ -3613,7 +3601,7 @@
         <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3">
         <v>169321</v>
@@ -3648,7 +3636,7 @@
         <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>74007</v>
@@ -3683,7 +3671,7 @@
         <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5">
         <v>142186</v>
@@ -3718,7 +3706,7 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6">
         <v>15758</v>
@@ -3750,10 +3738,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C7">
         <v>4928</v>
@@ -3788,7 +3776,7 @@
         <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8">
         <v>15753</v>
@@ -3820,10 +3808,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9">
         <v>7965</v>
@@ -3858,7 +3846,7 @@
         <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10">
         <v>37465</v>
@@ -3893,7 +3881,7 @@
         <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C11">
         <v>31047</v>
@@ -3928,7 +3916,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12">
         <v>70424</v>
@@ -3995,10 +3983,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14">
         <v>72264</v>
@@ -4033,7 +4021,7 @@
         <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C15">
         <v>88684</v>
@@ -4103,7 +4091,7 @@
         <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17">
         <v>133283</v>
@@ -4138,7 +4126,7 @@
         <v>141</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18">
         <v>26506</v>
@@ -4208,7 +4196,7 @@
         <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C20">
         <v>32472</v>
@@ -4243,7 +4231,7 @@
         <v>143</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C21">
         <v>250527</v>
@@ -4278,7 +4266,7 @@
         <v>144</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C22">
         <v>38558</v>
@@ -4313,7 +4301,7 @@
         <v>145</v>
       </c>
       <c r="B23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C23">
         <v>72959</v>
@@ -4348,7 +4336,7 @@
         <v>146</v>
       </c>
       <c r="B24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24">
         <v>20811</v>
@@ -4380,10 +4368,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25">
         <v>6757</v>
@@ -4418,7 +4406,7 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C26">
         <v>34532</v>
@@ -4453,7 +4441,7 @@
         <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27">
         <v>101491</v>
@@ -4488,7 +4476,7 @@
         <v>148</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C28">
         <v>36096</v>
@@ -4523,7 +4511,7 @@
         <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C29">
         <v>156677</v>
@@ -4558,7 +4546,7 @@
         <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C30">
         <v>63140</v>
@@ -4593,7 +4581,7 @@
         <v>129</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C31">
         <v>86034</v>
@@ -4695,10 +4683,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34">
         <v>9918</v>
@@ -4730,10 +4718,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C35">
         <v>37033</v>
@@ -4768,7 +4756,7 @@
         <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -4803,7 +4791,7 @@
         <v>153</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -4835,10 +4823,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -4870,10 +4858,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -4905,7 +4893,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B40" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
update figure 4 category names
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\selva\Documents\Coding\EPQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF22FE8-1E41-467D-BDFD-0DA9E6FFBB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B4FF0C-29F1-405B-BB4C-12795C9E3540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{92BFCFC7-AC86-46C9-9D17-467961656618}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{92BFCFC7-AC86-46C9-9D17-467961656618}"/>
   </bookViews>
   <sheets>
     <sheet name="admissions" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="198">
   <si>
     <t>QueenMary, University of Lon.. Other Russell Group</t>
   </si>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>Welsh: second language</t>
+  </si>
+  <si>
+    <t>Languages (excl. first language)</t>
   </si>
 </sst>
 </file>
@@ -723,17 +726,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1176,8 +1177,7 @@
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="3"/>
     </row>
   </sheetData>
@@ -1218,10 +1218,10 @@
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>-10.828094482421875</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>1.9713782072067261</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1232,10 +1232,10 @@
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>-1.7365915775299072</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1.0964227914810181</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1246,10 +1246,10 @@
       <c r="A4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>15.344949722290039</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1.5937222242355347</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1260,10 +1260,10 @@
       <c r="A5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>-5.4899263381958008</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1.0641186237335205</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1274,10 +1274,10 @@
       <c r="A6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>17.184593200683594</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>1.0305472612380981</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1288,10 +1288,10 @@
       <c r="A7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>-0.45530495047569275</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>1.5636910200119019</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1302,10 +1302,10 @@
       <c r="A8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>2.1625204086303711</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>1.0903264284133911</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1316,10 +1316,10 @@
       <c r="A9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>18.711397171020508</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>1.3240159749984741</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1330,10 +1330,10 @@
       <c r="A10" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>-10.855645179748535</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.82732939720153809</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1344,10 +1344,10 @@
       <c r="A11" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>36.504833221435547</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>1.7760151624679565</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1358,10 +1358,10 @@
       <c r="A12" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>-2.3518533706665039</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1.0113992691040039</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1372,10 +1372,10 @@
       <c r="A13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>15.286249160766602</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>1.2662296295166016</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1386,10 +1386,10 @@
       <c r="A14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>-6.5423569679260254</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>0.90979486703872681</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1400,10 +1400,10 @@
       <c r="A15" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>2.4479572772979736</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>1.1499499082565308</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1414,10 +1414,10 @@
       <c r="A16" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>0</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1428,10 +1428,10 @@
       <c r="A17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>-6.5887532234191895</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>1.0530462265014648</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1442,10 +1442,10 @@
       <c r="A18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>15.322231292724609</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>1.1343294382095337</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1456,10 +1456,10 @@
       <c r="A19" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>13.004060745239258</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>1.5071463584899902</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1470,10 +1470,10 @@
       <c r="A20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>30.390087127685547</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>1.7356675863265991</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1484,10 +1484,10 @@
       <c r="A21" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>-2.2864956855773926</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>1.576213002204895</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1498,10 +1498,10 @@
       <c r="A22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>6.8605880737304688</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>2.0234951972961426</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1512,10 +1512,10 @@
       <c r="A23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>-9.6349172592163086</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>1.397850513458252</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1526,10 +1526,10 @@
       <c r="A24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>0.74585658311843872</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>1.7692694664001465</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1540,10 +1540,10 @@
       <c r="A25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>-2.9467265605926514</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>1.4011307954788208</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1554,10 +1554,10 @@
       <c r="A26" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>8.4378700256347656</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>1.3458186388015747</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1568,10 +1568,10 @@
       <c r="A27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>-6.7986283302307129</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>0.95078802108764648</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1582,10 +1582,10 @@
       <c r="A28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>-14.583863258361816</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>1.662558913230896</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1596,10 +1596,10 @@
       <c r="A29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>-4.2522740364074707</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>0.98858988285064697</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1610,10 +1610,10 @@
       <c r="A30" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>5.5515217781066895</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>1.1802462339401245</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -1624,10 +1624,10 @@
       <c r="A31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>2.6612999439239502</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>1.9633474349975586</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1638,10 +1638,10 @@
       <c r="A32" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>-11.835053443908691</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>2.9633908271789551</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8DA5E3-C5AF-4EA3-A423-ADB8D65E05D0}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1680,7 @@
       <c r="D1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1691,10 +1691,10 @@
       <c r="B2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>0.29499999999999998</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>0.13800000000000001</v>
       </c>
       <c r="E2" s="2">
@@ -1708,10 +1708,10 @@
       <c r="B3" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0.25700000000000001</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.18</v>
       </c>
       <c r="E3" s="2">
@@ -1725,10 +1725,10 @@
       <c r="B4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0.246</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>0.16400000000000001</v>
       </c>
       <c r="E4" s="2">
@@ -1742,10 +1742,10 @@
       <c r="B5" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0.25</v>
       </c>
       <c r="E5" s="2">
@@ -1759,10 +1759,10 @@
       <c r="B6" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.20300000000000001</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>0.16400000000000001</v>
       </c>
       <c r="E6" s="2"/>
@@ -1774,10 +1774,10 @@
       <c r="B7" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.20100000000000001</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0.191</v>
       </c>
       <c r="E7" s="2"/>
@@ -1789,10 +1789,10 @@
       <c r="B8" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>0.2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>0.248</v>
       </c>
       <c r="E8" s="2"/>
@@ -1804,10 +1804,10 @@
       <c r="B9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0.16800000000000001</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>0.14499999999999999</v>
       </c>
       <c r="E9" s="2"/>
@@ -1819,10 +1819,10 @@
       <c r="B10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>0.161</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>0.42199999999999999</v>
       </c>
       <c r="E10" s="2"/>
@@ -1834,10 +1834,10 @@
       <c r="B11" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>0.151</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>0.13900000000000001</v>
       </c>
       <c r="E11" s="2"/>
@@ -1849,10 +1849,10 @@
       <c r="B12" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0.15</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0.35099999999999998</v>
       </c>
       <c r="E12" s="2"/>
@@ -1864,10 +1864,10 @@
       <c r="B13" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>0.13900000000000001</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>0.28899999999999998</v>
       </c>
       <c r="E13" s="2"/>
@@ -1879,10 +1879,10 @@
       <c r="B14" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0.13900000000000001</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>0.25600000000000001</v>
       </c>
       <c r="E14" s="2"/>
@@ -1894,10 +1894,10 @@
       <c r="B15" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0.13900000000000001</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>0.13200000000000001</v>
       </c>
       <c r="E15" s="2"/>
@@ -1909,10 +1909,10 @@
       <c r="B16" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0.13100000000000001</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>0.11600000000000001</v>
       </c>
       <c r="E16" s="2"/>
@@ -1924,10 +1924,10 @@
       <c r="B17" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>0.126</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>0.13500000000000001</v>
       </c>
       <c r="E17" s="2"/>
@@ -1939,10 +1939,10 @@
       <c r="B18" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>0.124</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="E18" s="2"/>
@@ -1954,10 +1954,10 @@
       <c r="B19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>0.10299999999999999</v>
       </c>
       <c r="E19" s="2"/>
@@ -1969,10 +1969,10 @@
       <c r="B20" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>0.375</v>
       </c>
       <c r="E20" s="2"/>
@@ -1984,10 +1984,10 @@
       <c r="B21" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>0.109</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>0.20799999999999999</v>
       </c>
       <c r="E21" s="2"/>
@@ -1999,10 +1999,10 @@
       <c r="B22" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>0.108</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>0.28699999999999998</v>
       </c>
       <c r="E22" s="2"/>
@@ -2014,10 +2014,10 @@
       <c r="B23" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>0.104</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>0.41899999999999998</v>
       </c>
       <c r="E23" s="2"/>
@@ -2029,10 +2029,10 @@
       <c r="B24" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>0.104</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>0.314</v>
       </c>
       <c r="E24" s="2"/>
@@ -2044,10 +2044,10 @@
       <c r="B25" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>0.104</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>0.28899999999999998</v>
       </c>
       <c r="E25" s="2"/>
@@ -2059,10 +2059,10 @@
       <c r="B26" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>0.1</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>0.16900000000000001</v>
       </c>
       <c r="E26" s="2"/>
@@ -2074,10 +2074,10 @@
       <c r="B27" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>0.122</v>
       </c>
       <c r="E27" s="2"/>
@@ -2089,10 +2089,10 @@
       <c r="B28" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="E28" s="2"/>
@@ -2104,10 +2104,10 @@
       <c r="B29" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>0.122</v>
       </c>
       <c r="E29" s="2"/>
@@ -2119,10 +2119,10 @@
       <c r="B30" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>0.25900000000000001</v>
       </c>
       <c r="E30" s="2"/>
@@ -2134,10 +2134,10 @@
       <c r="B31" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>0.13800000000000001</v>
       </c>
       <c r="E31" s="2"/>
@@ -2149,10 +2149,10 @@
       <c r="B32" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>0.189</v>
       </c>
       <c r="E32" s="2"/>
@@ -2164,10 +2164,10 @@
       <c r="B33" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>0.153</v>
       </c>
       <c r="E33" s="2"/>
@@ -2179,10 +2179,10 @@
       <c r="B34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>0.108</v>
       </c>
       <c r="E34" s="2"/>
@@ -2194,10 +2194,10 @@
       <c r="B35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>0.16600000000000001</v>
       </c>
       <c r="E35" s="2"/>
@@ -2209,10 +2209,10 @@
       <c r="B36" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>0.14399999999999999</v>
       </c>
       <c r="E36" s="2"/>
@@ -2224,10 +2224,10 @@
       <c r="B37" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>0.106</v>
       </c>
       <c r="E37" s="2"/>
@@ -2239,10 +2239,10 @@
       <c r="B38" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>0.17</v>
       </c>
       <c r="E38" s="2"/>
@@ -2254,10 +2254,10 @@
       <c r="B39" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <v>0.11899999999999999</v>
       </c>
       <c r="E39" s="2"/>
@@ -2269,10 +2269,10 @@
       <c r="B40" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="E40" s="2"/>
@@ -2284,10 +2284,10 @@
       <c r="B41" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="6">
         <v>0.16700000000000001</v>
       </c>
       <c r="E41" s="2"/>
@@ -2299,10 +2299,10 @@
       <c r="B42" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="6">
         <v>0.06</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="6">
         <v>0.23699999999999999</v>
       </c>
       <c r="E42" s="2"/>
@@ -2314,10 +2314,10 @@
       <c r="B43" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="6">
         <v>0.06</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="6">
         <v>0.115</v>
       </c>
       <c r="E43" s="2"/>
@@ -2329,10 +2329,10 @@
       <c r="B44" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="6">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="6">
         <v>0.498</v>
       </c>
       <c r="E44" s="2"/>
@@ -2344,10 +2344,10 @@
       <c r="B45" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>0.29499999999999998</v>
       </c>
       <c r="E45" s="2"/>
@@ -2359,10 +2359,10 @@
       <c r="B46" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="6">
         <v>0.19800000000000001</v>
       </c>
       <c r="E46" s="2"/>
@@ -2374,10 +2374,10 @@
       <c r="B47" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>0.13300000000000001</v>
       </c>
       <c r="E47" s="2"/>
@@ -2389,10 +2389,10 @@
       <c r="B48" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="6">
         <v>0.05</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="6">
         <v>0.151</v>
       </c>
       <c r="E48" s="2"/>
@@ -2404,10 +2404,10 @@
       <c r="B49" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="6">
         <v>0.21</v>
       </c>
       <c r="E49" s="2"/>
@@ -2419,10 +2419,10 @@
       <c r="B50" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="6">
         <v>0.14899999999999999</v>
       </c>
       <c r="E50" s="2"/>
@@ -2434,10 +2434,10 @@
       <c r="B51" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>4.7E-2</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="6">
         <v>0.17699999999999999</v>
       </c>
       <c r="E51" s="2"/>
@@ -2449,10 +2449,10 @@
       <c r="B52" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="6">
         <v>4.7E-2</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="6">
         <v>6.3E-2</v>
       </c>
       <c r="E52" s="2"/>
@@ -2464,10 +2464,10 @@
       <c r="B53" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="6">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="6">
         <v>0.61099999999999999</v>
       </c>
       <c r="E53" s="2">
@@ -2481,10 +2481,10 @@
       <c r="B54" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="6">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="6">
         <v>0.27600000000000002</v>
       </c>
       <c r="E54" s="2"/>
@@ -2496,10 +2496,10 @@
       <c r="B55" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="6">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="6">
         <v>0.22900000000000001</v>
       </c>
       <c r="E55" s="2"/>
@@ -2511,10 +2511,10 @@
       <c r="B56" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="6">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="6">
         <v>0.153</v>
       </c>
       <c r="E56" s="2"/>
@@ -2526,10 +2526,10 @@
       <c r="B57" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="6">
         <v>0.45500000000000002</v>
       </c>
       <c r="E57" s="2"/>
@@ -2541,10 +2541,10 @@
       <c r="B58" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="6">
         <v>0.184</v>
       </c>
       <c r="E58" s="2"/>
@@ -2556,10 +2556,10 @@
       <c r="B59" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="6">
         <v>0.1</v>
       </c>
       <c r="E59" s="2"/>
@@ -2571,10 +2571,10 @@
       <c r="B60" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="6">
         <v>0.60299999999999998</v>
       </c>
       <c r="E60" s="2">
@@ -2588,10 +2588,10 @@
       <c r="B61" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61" s="6">
         <v>0.314</v>
       </c>
       <c r="E61" s="2"/>
@@ -2603,10 +2603,10 @@
       <c r="B62" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="6">
         <v>0.255</v>
       </c>
       <c r="E62" s="2"/>
@@ -2618,10 +2618,10 @@
       <c r="B63" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="6">
         <v>0.23</v>
       </c>
       <c r="E63" s="2"/>
@@ -2633,10 +2633,10 @@
       <c r="B64" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="6">
         <v>0.19900000000000001</v>
       </c>
       <c r="E64" s="2"/>
@@ -2648,10 +2648,10 @@
       <c r="B65" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="6">
         <v>0.29799999999999999</v>
       </c>
       <c r="E65" s="2"/>
@@ -2663,10 +2663,10 @@
       <c r="B66" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="6">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="6">
         <v>0.16700000000000001</v>
       </c>
       <c r="E66" s="2"/>
@@ -2678,10 +2678,10 @@
       <c r="B67" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="6">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D67" s="6">
         <v>0.16500000000000001</v>
       </c>
       <c r="E67" s="2"/>
@@ -2693,10 +2693,10 @@
       <c r="B68" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="6">
         <v>0.36199999999999999</v>
       </c>
       <c r="E68" s="2"/>
@@ -2708,10 +2708,10 @@
       <c r="B69" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D69" s="6">
         <v>0.314</v>
       </c>
       <c r="E69" s="2"/>
@@ -2723,10 +2723,10 @@
       <c r="B70" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D70" s="6">
         <v>0.155</v>
       </c>
       <c r="E70" s="2"/>
@@ -2738,10 +2738,10 @@
       <c r="B71" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D71" s="7">
+      <c r="D71" s="6">
         <v>0.38400000000000001</v>
       </c>
       <c r="E71" s="2"/>
@@ -2753,10 +2753,10 @@
       <c r="B72" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72" s="6">
         <v>0.26400000000000001</v>
       </c>
       <c r="E72" s="2"/>
@@ -2768,10 +2768,10 @@
       <c r="B73" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="6">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="E73" s="2"/>
@@ -2783,10 +2783,10 @@
       <c r="B74" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="6">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="6">
         <v>0.217</v>
       </c>
       <c r="E74" s="2"/>
@@ -2798,10 +2798,10 @@
       <c r="B75" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="6">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="6">
         <v>0.4</v>
       </c>
       <c r="E75" s="2"/>
@@ -2813,10 +2813,10 @@
       <c r="B76" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="6">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="6">
         <v>0.107</v>
       </c>
       <c r="E76" s="2"/>
@@ -2828,10 +2828,10 @@
       <c r="B77" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="6">
         <v>0.32500000000000001</v>
       </c>
       <c r="E77" s="2"/>
@@ -2843,10 +2843,10 @@
       <c r="B78" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="6">
         <v>0.30099999999999999</v>
       </c>
       <c r="E78" s="2"/>
@@ -2858,10 +2858,10 @@
       <c r="B79" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D79" s="6">
         <v>0.20699999999999999</v>
       </c>
       <c r="E79" s="2"/>
@@ -2873,10 +2873,10 @@
       <c r="B80" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="6">
         <v>0.13200000000000001</v>
       </c>
       <c r="E80" s="2"/>
@@ -2888,10 +2888,10 @@
       <c r="B81" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D81" s="6">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="E81" s="2"/>
@@ -2903,10 +2903,10 @@
       <c r="B82" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="6">
         <v>0.03</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D82" s="6">
         <v>0.184</v>
       </c>
       <c r="E82" s="2"/>
@@ -2918,10 +2918,10 @@
       <c r="B83" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D83" s="6">
         <v>0.34300000000000003</v>
       </c>
       <c r="E83" s="2"/>
@@ -2933,10 +2933,10 @@
       <c r="B84" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D84" s="6">
         <v>0.192</v>
       </c>
       <c r="E84" s="2"/>
@@ -2948,10 +2948,10 @@
       <c r="B85" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D85" s="6">
         <v>0.182</v>
       </c>
       <c r="E85" s="2"/>
@@ -2963,10 +2963,10 @@
       <c r="B86" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D86" s="6">
         <v>0.36199999999999999</v>
       </c>
       <c r="E86" s="2"/>
@@ -2978,10 +2978,10 @@
       <c r="B87" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D87" s="6">
         <v>0.22700000000000001</v>
       </c>
       <c r="E87" s="2"/>
@@ -2993,10 +2993,10 @@
       <c r="B88" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C88" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D88" s="6">
         <v>0.23699999999999999</v>
       </c>
       <c r="E88" s="2"/>
@@ -3008,10 +3008,10 @@
       <c r="B89" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D89" s="6">
         <v>0.16700000000000001</v>
       </c>
       <c r="E89" s="2"/>
@@ -3023,10 +3023,10 @@
       <c r="B90" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D90" s="6">
         <v>0.32500000000000001</v>
       </c>
       <c r="E90" s="2"/>
@@ -3038,10 +3038,10 @@
       <c r="B91" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D91" s="6">
         <v>0.24399999999999999</v>
       </c>
       <c r="E91" s="2"/>
@@ -3053,10 +3053,10 @@
       <c r="B92" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C92" s="7">
+      <c r="C92" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D92" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="E92" s="2"/>
@@ -3068,10 +3068,10 @@
       <c r="B93" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C93" s="7">
+      <c r="C93" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="D93" s="7">
+      <c r="D93" s="6">
         <v>0.40899999999999997</v>
       </c>
       <c r="E93" s="2"/>
@@ -3083,10 +3083,10 @@
       <c r="B94" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C94" s="7">
+      <c r="C94" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D94" s="6">
         <v>0.23799999999999999</v>
       </c>
       <c r="E94" s="2"/>
@@ -3098,10 +3098,10 @@
       <c r="B95" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C95" s="7">
+      <c r="C95" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="D95" s="7">
+      <c r="D95" s="6">
         <v>0.104</v>
       </c>
       <c r="E95" s="2"/>
@@ -3113,10 +3113,10 @@
       <c r="B96" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="D96" s="7">
+      <c r="D96" s="6">
         <v>0.1</v>
       </c>
       <c r="E96" s="2"/>
@@ -3128,10 +3128,10 @@
       <c r="B97" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C97" s="7">
+      <c r="C97" s="6">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D97" s="7">
+      <c r="D97" s="6">
         <v>0</v>
       </c>
       <c r="E97" s="2"/>
@@ -3143,10 +3143,10 @@
       <c r="B98" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C98" s="7">
+      <c r="C98" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="D98" s="7">
+      <c r="D98" s="6">
         <v>0.33800000000000002</v>
       </c>
       <c r="E98" s="2"/>
@@ -3158,10 +3158,10 @@
       <c r="B99" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="D99" s="7">
+      <c r="D99" s="6">
         <v>0.32</v>
       </c>
       <c r="E99" s="2"/>
@@ -3173,10 +3173,10 @@
       <c r="B100" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C100" s="7">
+      <c r="C100" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="D100" s="7">
+      <c r="D100" s="6">
         <v>0.42199999999999999</v>
       </c>
       <c r="E100" s="2"/>
@@ -3188,10 +3188,10 @@
       <c r="B101" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C101" s="7">
+      <c r="C101" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D101" s="7">
+      <c r="D101" s="6">
         <v>0.46100000000000002</v>
       </c>
       <c r="E101" s="2"/>
@@ -3203,10 +3203,10 @@
       <c r="B102" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C102" s="7">
+      <c r="C102" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D102" s="7">
+      <c r="D102" s="6">
         <v>0.39800000000000002</v>
       </c>
       <c r="E102" s="2"/>
@@ -3218,10 +3218,10 @@
       <c r="B103" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C103" s="7">
+      <c r="C103" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D103" s="7">
+      <c r="D103" s="6">
         <v>0.36799999999999999</v>
       </c>
       <c r="E103" s="2"/>
@@ -3233,10 +3233,10 @@
       <c r="B104" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C104" s="7">
+      <c r="C104" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="D104" s="7">
+      <c r="D104" s="6">
         <v>0.38800000000000001</v>
       </c>
       <c r="E104" s="2"/>
@@ -3248,10 +3248,10 @@
       <c r="B105" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C105" s="7">
+      <c r="C105" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D105" s="7">
+      <c r="D105" s="6">
         <v>0.625</v>
       </c>
       <c r="E105" s="2">
@@ -3265,10 +3265,10 @@
       <c r="B106" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C106" s="7">
+      <c r="C106" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="D106" s="7">
+      <c r="D106" s="6">
         <v>0.48899999999999999</v>
       </c>
       <c r="E106" s="2"/>
@@ -3280,10 +3280,10 @@
       <c r="B107" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C107" s="7">
+      <c r="C107" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="D107" s="7">
+      <c r="D107" s="6">
         <v>0.28399999999999997</v>
       </c>
       <c r="E107" s="2"/>
@@ -3295,10 +3295,10 @@
       <c r="B108" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C108" s="7">
+      <c r="C108" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="D108" s="7">
+      <c r="D108" s="6">
         <v>0.26200000000000001</v>
       </c>
       <c r="E108" s="2"/>
@@ -3310,10 +3310,10 @@
       <c r="B109" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C109" s="7">
+      <c r="C109" s="6">
         <v>0.01</v>
       </c>
-      <c r="D109" s="7">
+      <c r="D109" s="6">
         <v>0.54400000000000004</v>
       </c>
       <c r="E109" s="2">
@@ -3327,10 +3327,10 @@
       <c r="B110" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C110" s="7">
+      <c r="C110" s="6">
         <v>0.01</v>
       </c>
-      <c r="D110" s="7">
+      <c r="D110" s="6">
         <v>0.42299999999999999</v>
       </c>
       <c r="E110" s="2"/>
@@ -3342,10 +3342,10 @@
       <c r="B111" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C111" s="7">
+      <c r="C111" s="6">
         <v>0.01</v>
       </c>
-      <c r="D111" s="7">
+      <c r="D111" s="6">
         <v>0.36799999999999999</v>
       </c>
       <c r="E111" s="2"/>
@@ -3357,10 +3357,10 @@
       <c r="B112" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C112" s="7">
+      <c r="C112" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D112" s="7">
+      <c r="D112" s="6">
         <v>0.59</v>
       </c>
       <c r="E112" s="2">
@@ -3520,11 +3520,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D47377-8598-4870-8D88-006F9A53E6A9}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3951,7 +3955,7 @@
         <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C13">
         <v>28214</v>
@@ -4056,7 +4060,7 @@
         <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C16">
         <v>11380</v>
@@ -4161,7 +4165,7 @@
         <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C19">
         <v>774</v>
@@ -4616,7 +4620,7 @@
         <v>150</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C32">
         <v>21559</v>
@@ -4651,7 +4655,7 @@
         <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C33">
         <v>19389</v>
@@ -4896,7 +4900,7 @@
         <v>196</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C40">
         <v>0</v>

</xml_diff>